<commit_message>
Add new Data Cleaning and Excel Charts tutorial files; update NashvilleHousing SQL script
</commit_message>
<xml_diff>
--- a/Excel/Conditional Formatting Excel Tutorial File.xlsx
+++ b/Excel/Conditional Formatting Excel Tutorial File.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\sql_practice\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE12AABD-2C2A-4D60-B298-E861FD33474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DD7103-7433-482A-B665-EE80A73E0A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="Sales" sheetId="4" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Demographics!$A$1:$K$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -333,8 +336,163 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFF6C0A2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -347,9 +505,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,7 +545,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -493,7 +651,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -635,7 +793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -646,25 +804,25 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.76171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.64453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.76171875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.52734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.52734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,91 +857,91 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H2">
-        <v>45000</v>
+        <v>50000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>65000</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>1001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4">
         <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>36000</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4">
-        <v>29</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -792,124 +950,124 @@
         <v>13</v>
       </c>
       <c r="H4">
-        <v>63000</v>
+        <v>45000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5">
         <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5">
-        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>47000</v>
+        <v>36000</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="H6">
-        <v>50000</v>
+        <v>63000</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H7">
-        <v>65000</v>
+        <v>47000</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -944,7 +1102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -979,7 +1137,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1014,20 +1172,34 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D22" t="str">
         <f t="shared" ref="D22:D23" si="0">CONCATENATE(B12," ",C12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{1027015F-D30F-450C-928C-DE78480974B7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K10">
+      <sortCondition sortBy="cellColor" ref="I1" dxfId="9"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="H2:H10">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>H2:H10&gt;50000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I10">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1035,16 +1207,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CCAA7F-6F85-4102-B7D4-D80770622F9F}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>72</v>
       </c>
@@ -1082,7 +1254,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1123,7 +1295,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1164,7 +1336,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1206,6 +1378,24 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:M2">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:M3">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>